<commit_message>
Updated both data frames
</commit_message>
<xml_diff>
--- a/CallTranscript_DownloadTemplate.xlsx
+++ b/CallTranscript_DownloadTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9238603-FD1F-49BC-9F42-1EC893FF77F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2169FB-8476-4DF9-8C50-24C5E712208A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Ticker</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>STT</t>
+  </si>
+  <si>
+    <t>q3</t>
   </si>
   <si>
     <t>q1</t>
@@ -385,7 +388,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,7 +409,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>2019</v>
@@ -420,7 +423,7 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -431,7 +434,7 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -442,7 +445,7 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -453,7 +456,7 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -464,7 +467,7 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -475,7 +478,7 @@
         <v>14</v>
       </c>
       <c r="C8">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -486,7 +489,7 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -497,7 +500,7 @@
         <v>14</v>
       </c>
       <c r="C10">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -508,7 +511,7 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -519,7 +522,7 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added data for 5 quarters 10 companies
</commit_message>
<xml_diff>
--- a/CallTranscript_DownloadTemplate.xlsx
+++ b/CallTranscript_DownloadTemplate.xlsx
@@ -1,18 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2169FB-8476-4DF9-8C50-24C5E712208A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akshitachawdhary/Desktop/DA_Davidson/Capstone_NLP_DIWD/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Ticker</t>
   </si>
@@ -31,40 +41,10 @@
     <t>Year</t>
   </si>
   <si>
-    <t>GOOG</t>
-  </si>
-  <si>
-    <t>GOOGL</t>
-  </si>
-  <si>
-    <t>GE</t>
-  </si>
-  <si>
-    <t>ETN</t>
-  </si>
-  <si>
-    <t>PEP</t>
-  </si>
-  <si>
     <t>KHC</t>
   </si>
   <si>
-    <t>FB</t>
-  </si>
-  <si>
     <t>MCHP</t>
-  </si>
-  <si>
-    <t>SLAB</t>
-  </si>
-  <si>
-    <t>JPM</t>
-  </si>
-  <si>
-    <t>STT</t>
-  </si>
-  <si>
-    <t>q3</t>
   </si>
   <si>
     <t>q1</t>
@@ -73,7 +53,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,16 +364,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,125 +384,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>2018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>